<commit_message>
"ajustes finais nos gráficos"
</commit_message>
<xml_diff>
--- a/resultados/comportamentoMMQ_preliminares.xlsx
+++ b/resultados/comportamentoMMQ_preliminares.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Logaritmo</t>
+          <t>Logarítmica</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -649,7 +649,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Logaritmo</t>
+          <t>Logarítmica</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -777,7 +777,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Logaritmo</t>
+          <t>Logarítmica</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Logaritmo</t>
+          <t>Logarítmica</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Logaritmo</t>
+          <t>Logarítmica</t>
         </is>
       </c>
       <c r="F19" t="n">

</xml_diff>